<commit_message>
u wont believe how far we've got
</commit_message>
<xml_diff>
--- a/billing/in/test.xlsx
+++ b/billing/in/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="rates" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,16 +31,16 @@
     <t xml:space="preserve">Scope</t>
   </si>
   <si>
+    <t xml:space="preserve">Valencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blood</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test</t>
   </si>
   <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valencia</t>
+    <t xml:space="preserve">ALL</t>
   </si>
 </sst>
 </file>
@@ -141,10 +141,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -161,19 +161,19 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
+      <c r="B2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>69</v>
@@ -183,14 +183,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,10 +219,6 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>